<commit_message>
modificaiones para simulaciones restantes
</commit_message>
<xml_diff>
--- a/Graficas.xlsx
+++ b/Graficas.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mis documentos\Desktop\SEMESTRE III\ALGORITMOS Y ESTRUCTURAS DE DATOS\HDT 5\Repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74F4B8D-73C5-4955-BF11-FDA2BABB12B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CDBE91-7E85-4A75-8C83-2860A6AD1AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B76EE2D5-465F-4EB6-94E8-1B049F4F9D7D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B76EE2D5-465F-4EB6-94E8-1B049F4F9D7D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulación original" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -437,7 +437,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Hoja1!$E$2:$E$6</c:f>
+                <c:f>'Simulación original'!$E$2:$E$6</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -461,7 +461,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Hoja1!$E$2:$E$6</c:f>
+                <c:f>'Simulación original'!$E$2:$E$6</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -499,7 +499,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>'Simulación original'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -523,7 +523,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$6</c:f>
+              <c:f>'Simulación original'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -717,7 +717,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-GT"/>
-                  <a:t>Tiempo promedio</a:t>
+                  <a:t>Tiempo promedio (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1129,7 +1129,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Hoja1!$E$7:$E$11</c:f>
+                <c:f>'Simulación original'!$E$7:$E$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1153,7 +1153,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Hoja1!$E$7:$E$11</c:f>
+                <c:f>'Simulación original'!$E$7:$E$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1191,7 +1191,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>'Simulación original'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1215,7 +1215,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$7:$C$11</c:f>
+              <c:f>'Simulación original'!$C$7:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1409,8 +1409,20 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-GT"/>
-                  <a:t>Tiempo promedio</a:t>
+                  <a:t>Tiempo promedio </a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="es-GT" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-GT"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1711,7 +1723,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Hoja1!$E$12:$E$16</c:f>
+                <c:f>'Simulación original'!$E$12:$E$16</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1735,7 +1747,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Hoja1!$E$12:$E$16</c:f>
+                <c:f>'Simulación original'!$E$12:$E$16</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1773,7 +1785,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>'Simulación original'!$B$12:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1797,7 +1809,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$12:$C$16</c:f>
+              <c:f>'Simulación original'!$C$12:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1951,7 +1963,7 @@
         <c:axId val="1276592751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="150"/>
+          <c:max val="200"/>
           <c:min val="24"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1991,8 +2003,20 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-GT"/>
-                  <a:t>Tiempo promedio</a:t>
+                  <a:t>Tiempo promedio </a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="es-GT" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-GT"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2228,7 +2252,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>'Simulación original'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2252,7 +2276,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$6</c:f>
+              <c:f>'Simulación original'!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2313,7 +2337,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>'Simulación original'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2337,7 +2361,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$7:$C$11</c:f>
+              <c:f>'Simulación original'!$C$7:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2398,7 +2422,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>'Simulación original'!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2422,7 +2446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$12:$C$16</c:f>
+              <c:f>'Simulación original'!$C$12:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2612,8 +2636,20 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-GT"/>
-                  <a:t>Tiempo promedio</a:t>
+                  <a:t>Tiempo promedio </a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="es-GT" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-GT"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5306,8 +5342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E9FC91-A355-4E18-9CBA-065D5492EDF0}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="116" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>

</xml_diff>